<commit_message>
Upload laporan tubes via upload
</commit_message>
<xml_diff>
--- a/tugas/laporan.xlsx
+++ b/tugas/laporan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TUBESMBD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TUBESMBD\IF3144-1920\tugas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="5628" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8580" windowHeight="6480" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Tugas" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="37">
   <si>
     <t>advisor = 100, student = 100, section = 200,takes = 200</t>
   </si>
@@ -138,6 +138,15 @@
   </si>
   <si>
     <t>4. Lakukan pada setiap Query</t>
+  </si>
+  <si>
+    <t>SELECT name, dept_name FROM student WHERE tot_cred &gt; 30;</t>
+  </si>
+  <si>
+    <t>SELECT student.name,student.dept_name,takes.sec_id AS pengambilan,takes.semester,section.room_number,section.building,course.course_id,course.dept_name FROM takes JOIN student ON takes.ID = student.ID JOIN section ON takes.course_id = section.course_id JOIN course ON section.course_id = course.course_id;</t>
+  </si>
+  <si>
+    <t>ning</t>
   </si>
 </sst>
 </file>
@@ -518,7 +527,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C28"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -668,9 +677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -681,7 +688,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -700,10 +707,12 @@
         <v>0</v>
       </c>
       <c r="B4" s="3">
-        <f>0.09*1000</f>
-        <v>90</v>
-      </c>
-      <c r="C4" s="3"/>
+        <f>0.02*1000</f>
+        <v>20</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -713,17 +722,20 @@
         <f>0.02*1000</f>
         <v>20</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="3">
-        <f>0.05*1000</f>
-        <v>50</v>
-      </c>
-      <c r="C6" s="3"/>
+        <v>120</v>
+      </c>
+      <c r="C6" s="3">
+        <v>40</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
@@ -762,9 +774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -794,29 +804,34 @@
         <v>0</v>
       </c>
       <c r="B4" s="3">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3"/>
+        <f>0.06*1000</f>
+        <v>60</v>
+      </c>
+      <c r="C4" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="3">
-        <f>0.03*1000</f>
-        <v>30</v>
-      </c>
-      <c r="C5" s="3"/>
+        <v>70</v>
+      </c>
+      <c r="C5" s="3">
+        <v>20</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="3">
-        <f>0.08*1000</f>
-        <v>80</v>
-      </c>
-      <c r="C6" s="3"/>
+        <v>120</v>
+      </c>
+      <c r="C6" s="3">
+        <v>50</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
@@ -855,9 +870,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -868,7 +881,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -889,7 +902,9 @@
       <c r="B4" s="3">
         <v>0</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -898,7 +913,9 @@
       <c r="B5" s="3">
         <v>0</v>
       </c>
-      <c r="C5" s="3"/>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
@@ -907,7 +924,9 @@
       <c r="B6" s="3">
         <v>0</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
@@ -946,9 +965,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
@@ -978,27 +995,34 @@
         <v>0</v>
       </c>
       <c r="B4" s="3">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3"/>
+        <f>0.07*1000</f>
+        <v>70</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="3">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="3">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3"/>
+        <v>60</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
@@ -1037,8 +1061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1071,16 +1095,20 @@
       <c r="B4" s="3">
         <v>0</v>
       </c>
-      <c r="C4" s="3"/>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="3">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
@@ -1089,7 +1117,9 @@
       <c r="B6" s="3">
         <v>0</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
@@ -1127,7 +1157,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
@@ -1195,6 +1225,11 @@
         <v>27</v>
       </c>
     </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Pengumpulan Laporan Praktikum MBD
</commit_message>
<xml_diff>
--- a/tugas/laporan.xlsx
+++ b/tugas/laporan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karunia/Documents/lecturer - DBMS/2019:2020/IF3144-1920/tugas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\#RIGBY MULTIMEDIA\Documents\A Tubes MBD\IF3144-1920-master\tugas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F409652C-A4B2-B041-93C9-55CCCBF85C91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1EE7EEE-FF8F-405E-8CB5-8CF6FAFC97B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16460" xr2:uid="{3C9D5799-7662-CB47-8B99-82C16436D226}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3C9D5799-7662-CB47-8B99-82C16436D226}"/>
   </bookViews>
   <sheets>
     <sheet name="Tugas" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>advisor = 100, student = 100, section = 200,takes = 200</t>
   </si>
@@ -73,18 +73,6 @@
     <t>SELECT * FROM student WHERE tot_cred &gt; 30;</t>
   </si>
   <si>
-    <t>SELECT * FROM student</t>
-  </si>
-  <si>
-    <t>SELECT `name`, department FROM student WHERE tot_cred &gt; 30;</t>
-  </si>
-  <si>
-    <t>SELECT *  FROM takes JOIN student ON takes.ID = student.ID JOIN section ON takes.course_id = section.course_id</t>
-  </si>
-  <si>
-    <t>SELECT student.`name`,student.dept_name,takes.sec_id AS pengambilan,takes.semester,section.room_number,section.building,course.course_id,course.dept_name FROM takes JOIN student ON takes.ID = student.ID JOIN section ON takes.course_id = section.course_id JOIN course ON section.course_id = course.course_id</t>
-  </si>
-  <si>
     <t>1. Run dengan menggunakan terminal Query di atas dan catat waktunya</t>
   </si>
   <si>
@@ -134,6 +122,36 @@
   </si>
   <si>
     <t>4. Lakukan pada setiap Query</t>
+  </si>
+  <si>
+    <t>SELECT `name`, dept_name FROM student WHERE tot_cred &gt; 30;</t>
+  </si>
+  <si>
+    <t>SELECT * FROM student;</t>
+  </si>
+  <si>
+    <t>SELECT *  FROM takes JOIN student ON takes.ID = student.ID JOIN section ON takes.course_id = section.course_id;</t>
+  </si>
+  <si>
+    <t>SELECT student.`name`,student.dept_name,takes.sec_id AS pengambilan,takes.semester,section.room_number,section.building,course.course_id,course.dept_name FROM takes JOIN student ON takes.ID = student.ID JOIN section ON takes.course_id = section.course_id JOIN course ON section.course_id = course.course_id;</t>
+  </si>
+  <si>
+    <t>1; 2; 1; 88; 4</t>
+  </si>
+  <si>
+    <t>2; 2; 2; 18; 12</t>
+  </si>
+  <si>
+    <t>55; 2; 3; 39; 102</t>
+  </si>
+  <si>
+    <t>1; 1; 1; 8; 7 | 0; 1; 0; 27; 2</t>
+  </si>
+  <si>
+    <t>2; 2; 1; 16; 12 | 1; 1; 1; 5; 4</t>
+  </si>
+  <si>
+    <t>3; 3; 2; 41; 33 | 1; 1; 1; 21; 15</t>
   </si>
 </sst>
 </file>
@@ -192,12 +210,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,18 +533,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7283ED88-C5BB-2349-93B1-5D98200E2DE2}">
   <dimension ref="A2:C28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.5" customWidth="1"/>
-    <col min="3" max="3" width="26.83203125" customWidth="1"/>
+    <col min="3" max="3" width="26.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -536,123 +555,135 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -665,69 +696,69 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B6" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B7" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B9" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B10" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pengumpulan Tugas Besar MBD
</commit_message>
<xml_diff>
--- a/tugas/laporan.xlsx
+++ b/tugas/laporan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karunia/Documents/lecturer - DBMS/2019:2020/IF3144-1920/tugas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Downloads\IF3144-1920-master\tugas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F409652C-A4B2-B041-93C9-55CCCBF85C91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B52EFF-2095-4D4F-AC82-B0175E10DB40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16460" xr2:uid="{3C9D5799-7662-CB47-8B99-82C16436D226}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{3C9D5799-7662-CB47-8B99-82C16436D226}"/>
   </bookViews>
   <sheets>
     <sheet name="Tugas" sheetId="1" r:id="rId1"/>
@@ -76,9 +76,6 @@
     <t>SELECT * FROM student</t>
   </si>
   <si>
-    <t>SELECT `name`, department FROM student WHERE tot_cred &gt; 30;</t>
-  </si>
-  <si>
     <t>SELECT *  FROM takes JOIN student ON takes.ID = student.ID JOIN section ON takes.course_id = section.course_id</t>
   </si>
   <si>
@@ -134,6 +131,9 @@
   </si>
   <si>
     <t>4. Lakukan pada setiap Query</t>
+  </si>
+  <si>
+    <t>SELECT dept_name FROM student WHERE tot_cred &gt; 30;</t>
   </si>
 </sst>
 </file>
@@ -514,18 +514,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7283ED88-C5BB-2349-93B1-5D98200E2DE2}">
   <dimension ref="A2:C28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView showGridLines="0" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="61.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.5" customWidth="1"/>
-    <col min="3" max="3" width="26.83203125" customWidth="1"/>
+    <col min="3" max="3" width="26.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -536,123 +536,123 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -664,70 +664,70 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EEE10EE-7B32-C94F-84A3-EE8D948576BC}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B6" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B7" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B9" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B10" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tugas Besar Manajemen Basisdata (finish)
</commit_message>
<xml_diff>
--- a/tugas/laporan.xlsx
+++ b/tugas/laporan.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karunia/Documents/lecturer - DBMS/2019:2020/IF3144-1920/tugas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\IF3144-1920-master\tugas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F409652C-A4B2-B041-93C9-55CCCBF85C91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16460" xr2:uid="{3C9D5799-7662-CB47-8B99-82C16436D226}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6105"/>
   </bookViews>
   <sheets>
     <sheet name="Tugas" sheetId="1" r:id="rId1"/>
     <sheet name="Laporan" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="40">
   <si>
     <t>advisor = 100, student = 100, section = 200,takes = 200</t>
   </si>
@@ -134,12 +133,30 @@
   </si>
   <si>
     <t>4. Lakukan pada setiap Query</t>
+  </si>
+  <si>
+    <t>QUERY 1</t>
+  </si>
+  <si>
+    <t>QUERY 2</t>
+  </si>
+  <si>
+    <t>QUERY 3</t>
+  </si>
+  <si>
+    <t>QUERY 4</t>
+  </si>
+  <si>
+    <t>QUERY 5</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -165,7 +182,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -188,16 +205,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,221 +561,466 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7283ED88-C5BB-2349-93B1-5D98200E2DE2}">
-  <dimension ref="A2:C28"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.5" customWidth="1"/>
-    <col min="3" max="3" width="26.83203125" customWidth="1"/>
+    <col min="1" max="1" width="61.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="8.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.375" customWidth="1"/>
+    <col min="8" max="8" width="7.75" customWidth="1"/>
+    <col min="9" max="9" width="7.625" customWidth="1"/>
+    <col min="10" max="11" width="8.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="B1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="B3" s="2">
+        <v>5.7710299999999999E-2</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3.678E-4</v>
+      </c>
+      <c r="D3" s="2">
+        <v>3.4909999999999997E-4</v>
+      </c>
+      <c r="E3" s="2">
+        <v>9.1142500000000001E-2</v>
+      </c>
+      <c r="F3" s="2">
+        <v>5.0515299999999999E-2</v>
+      </c>
+      <c r="G3" s="2">
+        <v>4.1110000000000002E-4</v>
+      </c>
+      <c r="H3" s="2">
+        <v>3.4600000000000001E-4</v>
+      </c>
+      <c r="I3" s="2">
+        <v>3.4309999999999999E-4</v>
+      </c>
+      <c r="J3" s="2">
+        <v>1.6470999999999999E-4</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1.4311E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="B4" s="2">
+        <v>4.6359999999999999E-4</v>
+      </c>
+      <c r="C4" s="2">
+        <v>6.2620000000000004E-4</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3.6143E-3</v>
+      </c>
+      <c r="E4" s="2">
+        <v>3.0785000000000001E-3</v>
+      </c>
+      <c r="F4" s="2">
+        <v>5.2360000000000004E-4</v>
+      </c>
+      <c r="G4" s="2">
+        <v>4.013E-4</v>
+      </c>
+      <c r="H4" s="2">
+        <v>4.7390000000000003E-4</v>
+      </c>
+      <c r="I4" s="2">
+        <v>4.0840000000000001E-4</v>
+      </c>
+      <c r="J4" s="2">
+        <v>3.7843E-3</v>
+      </c>
+      <c r="K4" s="2">
+        <v>2.9432E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
+      <c r="B5" s="2">
+        <v>8.2456600000000005E-2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>9.2960000000000004E-4</v>
+      </c>
+      <c r="D5" s="2">
+        <v>5.0060000000000002E-4</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.53413699999999997</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.56575640000000005</v>
+      </c>
+      <c r="G5" s="2">
+        <v>6.1359999999999995E-4</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.1314535</v>
+      </c>
+      <c r="I5" s="2">
+        <v>5.042E-4</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.62759430000000005</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0.33083810000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="B6" s="2">
+        <v>4.4920399999999999E-2</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3.3159999999999998E-4</v>
+      </c>
+      <c r="D6" s="2">
+        <v>3.6388000000000002E-4</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1.5384999999999999E-3</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2.6548000000000001E-3</v>
+      </c>
+      <c r="G6" s="2">
+        <v>3.4519999999999999E-4</v>
+      </c>
+      <c r="H6" s="2">
+        <v>3.4870000000000002E-4</v>
+      </c>
+      <c r="I6" s="2">
+        <v>3.1629999999999999E-4</v>
+      </c>
+      <c r="J6" s="2">
+        <v>9.7050999999999995E-3</v>
+      </c>
+      <c r="K6" s="2">
+        <v>1.4040000000000001E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="B7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="B8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="G1:K1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EEE10EE-7B32-C94F-84A3-EE8D948576BC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B6" s="4" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B7" s="4" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B9" s="4" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B10" s="4" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>27</v>
       </c>

</xml_diff>